<commit_message>
Adding flags and flag and location conditions; simplifying message processing; changing condition separator from | to &
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -87,13 +87,13 @@
   <si>
     <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
 "I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:name:pathtobaron}. You pass out.{|GOTO:pathtobaron|}
-You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby tree. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
+You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby TREE. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
   </si>
   <si>
     <t xml:space="preserve">MTM1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron|character:ranger</t>
+    <t xml:space="preserve">character:baron&amp;character:ranger</t>
   </si>
   <si>
     <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
@@ -139,6 +139,9 @@
     <t xml:space="preserve">BOTW1</t>
   </si>
   <si>
+    <t xml:space="preserve">character:baron&amp;character:ranger&amp;location:current:forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
 After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
   </si>
@@ -184,7 +187,7 @@
   </si>
   <si>
     <t xml:space="preserve">The next day, a small creature runs across your path. You almost step on it.
-You squat down to look at it. It seems like some sort of squirrel, but it's eyes are ruby red. It sits still, staring at you, alert.</t>
+You squat down to look at it. It seems like some sort of squirrel, but it's eyes are ruby red. It sits still, staring at you, alert.{|SET:squirrel:exists|}</t>
   </si>
   <si>
     <t xml:space="preserve">Give it some of your food</t>
@@ -193,7 +196,7 @@
     <t xml:space="preserve">Ignore it</t>
   </si>
   <si>
-    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into the {location:current:name}. </t>
+    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into {location:current:namewiththe}. </t>
   </si>
   <si>
     <t xml:space="preserve">The squirrel watches you as you leave, then scampers off.</t>
@@ -219,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve">ROT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest&amp;squirrel:exists</t>
   </si>
   <si>
     <t xml:space="preserve">You're being careful, but you don't notice a well-concealed pit before it's too late. You step through the thin covering of leaves and ferns and fall right through to the bottom, landing with a crunch.
@@ -288,7 +294,7 @@
     <t xml:space="preserve">AWF1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron|item:map</t>
+    <t xml:space="preserve">character:baron&amp;item:map</t>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into the Tower on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside the Tower.{|AWF1a|}</t>
@@ -297,7 +303,7 @@
     <t xml:space="preserve">AWF2</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron|item:map|character:stolen</t>
+    <t xml:space="preserve">character:baron&amp;item:map&amp;character:stolen</t>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into the Tower on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside the Tower. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
@@ -306,7 +312,7 @@
     <t xml:space="preserve">AWF3</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron|character:stolen</t>
+    <t xml:space="preserve">character:baron&amp;character:stolen</t>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling the Tower. You think you can find a way in between them, but it would be tough. What do you do?</t>
@@ -348,7 +354,7 @@
     <t xml:space="preserve">A1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:stolen|character:baron</t>
+    <t xml:space="preserve">character:stolen&amp;character:baron</t>
   </si>
   <si>
     <t xml:space="preserve">You find {character:stolen:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
@@ -745,8 +751,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -870,327 +876,324 @@
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allowing named locations to be used in messages
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="120">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -82,7 +82,7 @@
   </si>
   <si>
     <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for the Tower.{|GOTO:pathtobaron|}
-The next day, deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
   </si>
   <si>
     <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
@@ -106,12 +106,12 @@
     <t xml:space="preserve">Set off for the Tower (you know the way)</t>
   </si>
   <si>
-    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s Tower myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into {location:current:namewiththe}. {|GIVE:map:A cloth map:shows a hidden path into the Tower|}
+    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s Tower myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into the Tower|}
 The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s Tower. You roll it up again and put it in your pack.
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
-    <t xml:space="preserve">You walk further into {location:current:namewiththe}, headed for the Tower. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+    <t xml:space="preserve">You walk further into the {location:current:type}, headed for the Tower. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">Ignore it</t>
   </si>
   <si>
-    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into {location:current:namewiththe}. </t>
+    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into the {location:current:type}.</t>
   </si>
   <si>
     <t xml:space="preserve">The squirrel watches you as you leave, then scampers off.</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">ROT2</t>
   </si>
   <si>
-    <t xml:space="preserve">Late in the day, you hear a voice calling out through {location:current:namewiththe}. You hide immediately, but then realize the voice seems to be that of a young {character:child:sexAge:petowner}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
+    <t xml:space="preserve">Late in the day, you hear a voice calling out through the {location:current:type}. You hide immediately, but then realize the voice seems to be that of a young {character:child:sexAge:petowner}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Reveal yourself and offer to help</t>
@@ -241,7 +241,7 @@
 You fall a few times, but you make progress. The pain in your leg blends with the pain in the rest of your body. Very slowly, you make your way to the top. Your fingers are bleeding, your wrists hurt.</t>
   </si>
   <si>
-    <t xml:space="preserve">Your voice rings out into the {location:current:name}. No one answers.
+    <t xml:space="preserve">Your voice rings out into the {location:current:type}. No one answers.
 After a few minutes, you hear skittering and see the squirrel peek its head into view. Then it disappears.
 A minute later, a vine woven from ferns and grasses drops down into the pit with you. The squirrel reappears, it's red eyes flashing, before it disappears again.
 You climb easily out of the pit. The squirrel is nowhere to be seen.</t>
@@ -363,17 +363,23 @@
     <t xml:space="preserve">UB1</t>
   </si>
   <si>
-    <t xml:space="preserve">Searching in the Tower, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside the Tower. The {character:baron:baron}'s gold is gone. You leave the Tower.
-As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:current:name} as fast as you can.</t>
+    <t xml:space="preserve">Searching in the Tower, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside the Tower. The {character:baron:baron}'s gold is gone.</t>
   </si>
   <si>
     <t xml:space="preserve">ROR1</t>
   </si>
   <si>
+    <t xml:space="preserve">You leave the Tower.{|GOTO:pathtobaron|}</t>
+  </si>
+  <si>
     <t xml:space="preserve">MF1</t>
   </si>
   <si>
-    <t xml:space="preserve">The {character:baron:baron}'s men are chasing you through {location:pathtobaron:namewiththe} on your way back to {location:hometown:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
+    <t xml:space="preserve">character:baron&amp;location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:current:type} as fast as you can.
+The {character:baron:baron}'s men are chasing you through {location:pathtobaron:namewiththe} on your way back to {location:hometown:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
   </si>
   <si>
     <t xml:space="preserve">Spend your nights well-hidden, in a hole or under heavy brush</t>
@@ -751,8 +757,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1107,7 +1113,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -1118,82 +1124,88 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generating random fortress locations
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, the Tower. You know the way, which leads through the nearby {location:nearby:name:pathtobaron}.{|GOTO:pathtobaron|}
+    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:name:pathtobaron}.{|GOTO:pathtobaron|}
 Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
   </si>
   <si>
@@ -70,18 +70,68 @@
     <t xml:space="preserve">character:baron</t>
   </si>
   <si>
-    <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
 They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
-In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s Tower by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set out for the Tower immediately</t>
+In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{location:fortress:name:baronhome}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Set out for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{location:baronhome:namewiththe}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> immediately</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
   </si>
   <si>
-    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for the Tower.{|GOTO:pathtobaron|}
+    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}
 The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
   </si>
   <si>
@@ -97,28 +147,70 @@
   </si>
   <si>
     <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
-"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to the Tower."</t>
+"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
   </si>
   <si>
     <t xml:space="preserve">Ask {character:ranger:name} for {character:ranger:possPronoun} help</t>
   </si>
   <si>
-    <t xml:space="preserve">Set off for the Tower (you know the way)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s Tower myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into the Tower|}
-The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s Tower. You roll it up again and put it in your pack.
+    <t xml:space="preserve">Set off for {location:baronhome:namewiththe} (you know the way)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{location:baronhome:type:cap}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into the Tower|}
+The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{location:baronhome:type:cap}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. You roll it up again and put it in your pack.
 You travel through {location:current:namewiththe} for several days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk further into the {location:current:type}, headed for the Tower. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:baronhome:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
     <t xml:space="preserve">CTT1</t>
   </si>
   <si>
-    <t xml:space="preserve">A wide river blocks your path to the Tower. The water is deep and moving fast.</t>
+    <t xml:space="preserve">A wide river blocks your path to {location:baronhome:namewiththe}. The water is deep and moving fast.</t>
   </si>
   <si>
     <t xml:space="preserve">Wade through the rushing water</t>
@@ -129,11 +221,11 @@
   <si>
     <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
 It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
-Once you're ready, you continue on your way to the Tower.</t>
+Once you're ready, you continue on your way to {location:baronhome:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
-On the other side, you continue on your way to the Tower.</t>
+On the other side, you continue on your way to {location:baronhome:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">BOTW1</t>
@@ -175,12 +267,12 @@
   </si>
   <si>
     <t xml:space="preserve">It takes you over an hour, but you eventually feel the bonds loosening enough that you can slip out of them. The lone guard is still staring into the fire, poking at it with his sword and humming.
-You grab your pack silently and disappear into the night, using the stars to head in the direction of the Tower.</t>
+You grab your pack silently and disappear into the night, using the stars to head in the direction of {location:baronhome:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
 Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip into the night.
-You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward the Tower.</t>
+You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:baronhome:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">ROT1</t>
@@ -215,10 +307,10 @@
   </si>
   <si>
     <t xml:space="preserve">You step out from behind your tree, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
-Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to the Tower.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to the Tower.</t>
+Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">ROT3</t>
@@ -262,20 +354,20 @@
   <si>
     <t xml:space="preserve">"We're fighting against the {character:baron:baron}'s influence, to free the villages {character:baron:subPronoun}'s conquered from {character:baron:possPronoun} control." You share that you're trying to do the same thing.
 You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
-They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from the Tower, allowing you to get inside more easily.
-In the morning, you set off for the Tower again.</t>
+They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
+In the morning, you set off for {location:baronhome:namewiththe} again.</t>
   </si>
   <si>
     <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
 You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
-They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from the Tower, allowing you to get inside more easily.
-In the morning, you set off for the Tower again.</t>
+They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
+In the morning, you set off for {location:baronhome:namewiththe} again.</t>
   </si>
   <si>
     <t xml:space="preserve">WAT1</t>
   </si>
   <si>
-    <t xml:space="preserve">As you head towards the Tower, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
+    <t xml:space="preserve">As you head towards {location:baronhome:namewiththe}, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
   </si>
   <si>
     <t xml:space="preserve">Gather and enjoy some berries</t>
@@ -297,7 +389,7 @@
     <t xml:space="preserve">character:baron&amp;item:map</t>
   </si>
   <si>
-    <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into the Tower on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside the Tower.{|AWF1a|}</t>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}.{|AWF1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">AWF2</t>
@@ -306,7 +398,7 @@
     <t xml:space="preserve">character:baron&amp;item:map&amp;character:stolen</t>
   </si>
   <si>
-    <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into the Tower on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside the Tower. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">AWF3</t>
@@ -315,7 +407,7 @@
     <t xml:space="preserve">character:baron&amp;character:stolen</t>
   </si>
   <si>
-    <t xml:space="preserve">You finally arrive at the base of the Tower. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling the Tower. You think you can find a way in between them, but it would be tough. What do you do?</t>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling {location:baronhome:namewiththe}. You think you can find a way in between them, but it would be tough. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Sneak past the guards</t>
@@ -325,22 +417,22 @@
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
-Inside the Tower, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside the Tower in the gap in the patrol.
-Inside the Tower, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside {location:baronhome:namewiththe} in the gap in the patrol.
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">AWF4</t>
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
-Inside the Tower, you look around for the treasury. While you're looking, you hear voices.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside the Tower in the gap in the patrol.
-Inside the Tower, you look around for the treasury. While you're looking, you hear voices.{|AWF1a|}</t>
+Inside {location:baronhome:namewiththe}, you look around for the treasury. While you're looking, you hear voices.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside {location:baronhome:namewiththe} in the gap in the patrol.
+Inside {location:baronhome:namewiththe}, you look around for the treasury. While you're looking, you hear voices.{|AWF1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">AWF1a</t>
@@ -363,13 +455,13 @@
     <t xml:space="preserve">UB1</t>
   </si>
   <si>
-    <t xml:space="preserve">Searching in the Tower, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside the Tower. The {character:baron:baron}'s gold is gone.</t>
+    <t xml:space="preserve">Searching in {location:baronhome:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside {location:baronhome:namewiththe}. The {character:baron:baron}'s gold is gone.</t>
   </si>
   <si>
     <t xml:space="preserve">ROR1</t>
   </si>
   <si>
-    <t xml:space="preserve">You leave the Tower.{|GOTO:pathtobaron|}</t>
+    <t xml:space="preserve">You leave {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}</t>
   </si>
   <si>
     <t xml:space="preserve">MF1</t>
@@ -437,11 +529,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -457,6 +550,65 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -464,31 +616,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -496,42 +624,24 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -542,30 +652,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -583,6 +669,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -634,23 +744,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -669,23 +813,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -757,14 +901,14 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -811,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -834,7 +978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -857,7 +1001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Generating description of where the hometown is
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">CTA1</t>
   </si>
   <si>
-    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village on the edge of {location:hometown:feature:name}. You work on the fishing boats, bringing back enough fish each day to feed your small village.
+    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work on the fishing boats, bringing back enough fish each day to feed your small village.
 One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
 What do you do?</t>
   </si>
@@ -901,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adding industry replacements for towns
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">CTA1</t>
   </si>
   <si>
-    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work on the fishing boats, bringing back enough fish each day to feed your small village.
+    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, bringing back enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
 One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
 What do you do?</t>
   </si>
@@ -61,7 +61,7 @@
 Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
   </si>
   <si>
-    <t xml:space="preserve">The fish are biting, just like they always are this time of year. It's a good haul.{|ROC|}</t>
+    <t xml:space="preserve">{industry:hometown:goodday} {|ROC|}</t>
   </si>
   <si>
     <t xml:space="preserve">ROC1</t>
@@ -510,13 +510,13 @@
     <t xml:space="preserve">{location:hometown:name} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the Chief of {location:hometown:name}. What do you do?</t>
   </si>
   <si>
-    <t xml:space="preserve">Go back to your old job, fishing</t>
+    <t xml:space="preserve">Go back to your old job, {industry:hometown:workGer}</t>
   </si>
   <si>
     <t xml:space="preserve">Take the new job as Chief of {location:hometown:name}</t>
   </si>
   <si>
-    <t xml:space="preserve">The lake is peaceful and calm, and the fish are biting just like they always have. {location:hometown:name}'s freedom allows things to go back to the way that they were. But you know that, if ever another {character:baron:baron} tried to take control of {location:hometown:name} again, you and your neighbors would be ready for them.</t>
+    <t xml:space="preserve">{industry:hometown:gooddayfinal} {location:hometown:name}'s freedom allows things to go back to the way that they were. But you know that, if ever another {character:baron:baron} tried to take control of {location:hometown:name} again, you and your neighbors would be ready for them.</t>
   </si>
   <si>
     <t xml:space="preserve">Under your leadership, {location:hometown:name} is led to a new age of prosperity. You establish trade with other villages that were under {character:baron:baron} {character:baron:name}'s control. {location:hometown:name} thrives, and your people remain free and happy.</t>
@@ -901,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -935,7 +935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Adding ability to remove items and filter for if you DON'T have an item
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -68,6 +68,98 @@
   </si>
   <si>
     <t xml:space="preserve">character:baron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
+They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
+In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:fortress:name:baronhome} by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set out for {location:baronhome:namewiththe} immediately</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}
+The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
+"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:name:pathtobaron}. You pass out.{|GOTO:pathtobaron|}
+You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby TREE. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;character:ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
+"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask {character:ranger:name} for {character:ranger:possPronoun} help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set off for {location:baronhome:namewiththe} (you know the way)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s {location:baronhome:type:cap} myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into [location-baronhome-namewiththe]|}
+The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s {location:baronhome:type:cap}. You roll it up again and put it in your pack.
+You travel through {location:current:namewiththe} for several days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:baronhome:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+You travel through {location:current:namewiththe} for several days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A wide river blocks your path to {location:baronhome:namewiththe}. The water is deep and moving fast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wade through the rushing water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look for another way around</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
+It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
+Once you're ready, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
+On the other side, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A tall wall runs across your path to {location:baronhome:namewiththe}. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climb the wall here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking for a gap in the wall somewhere else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
+You continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further along the wall, you find a tall tree with a branch leaning over the wall. You climb the tree, edge out along the branch, and drop down on the other side of the wall.
+Once over the wall, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTW1</t>
   </si>
   <si>
     <r>
@@ -77,9 +169,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
-They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
-In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s </t>
+      <t xml:space="preserve">character:baron</t>
     </r>
     <r>
       <rPr>
@@ -87,8 +177,228 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:fortress:name:baronhome}</t>
+      <t xml:space="preserve">&amp;character:ranger&amp;location:current:forest</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
+After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide in the brush and wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek out the footsteps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You find a clump of bushes to hide inside. As the footsteps get closer, you see two dozen of the {character:baron:baron}'s armed men tramping through the underbrush.
+You hold your breath, but one of them stumbles just too close to you.
+"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the trees, two dozen of the {character:baron:baron}'s men in uniform emerge.
+One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTW1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp in the woods an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
+Most of them have fallen asleep, but there is still one awake, on guard, staring into the fire. He isn't looking directly at you, you could try to escape while he isn't looking. What do you do?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiggle out of your bonds and sneak into the night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait until morning for a chance to escape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It takes you over an hour, but you eventually feel the bonds loosening enough that you can slip out of them. The lone guard is still staring into the fire, poking at it with his sword and humming.
+You grab your pack silently and disappear into the night, using the stars to head in the direction of {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
+Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip into the night.
+You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTW2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
+After a day or so, it begins to rain heavily. You take shelter in a nearby cave, making your bed in a small alcove. You go to sleep to wait out the rain.
+When you wake up, you hear someone else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be getting ready to lie down. What do you do?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to scare them out of the cave so you can leave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait until they go to sleep, then sneak out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You get up suddenly, shouting and waving your arms threateningly.
+The bears are startled at first, but then rear up on their hind legs as well, roaring threateningly. They aren’t backing out, but they do leave you enough room to sneak between them, deftly dodging their sharp claws.
+You make it out, but the bears rip your pack off of your back. Your bedroll, all your food, and anything else you had in your pack is gone. You’ll have to forage for food and sleep on the ground from now on.{|REMOVE:map|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems like it takes an eternity, but eventually, as it’s getting dark outside again, the two bears settle down, nestled up against each other. You wait until you’re absolutely sure they’re asleep. Then, very, very quietly, you gather your bedroll and sneak past them out of the cave. The rain has stopped by now, and the {location:current:type} is quiet and dark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next day, a small creature runs across your path. You almost step on it.
+You squat down to look at it. It seems like some sort of squirrel, but it's eyes are ruby red. It sits still, staring at you, alert.{|SET:squirrel:exists|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give it some of your food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into the {location:current:type}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The squirrel watches you as you leave, then scampers off.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Late in the day, you hear a voice calling out through the {location:current:type}. You hide immediately, but then realize the voice seems to be that of a young {character:child:sexAge:petowner}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reveal yourself and offer to help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait until {character:petowner:subPronoun}'s gone and continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You step out from behind your tree, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
+Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location:current:forest&amp;squirrel:exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You're being careful, but you don't notice a well-concealed pit before it's too late. You step through the thin covering of leaves and ferns and fall right through to the bottom, landing with a crunch.
+Your leg hurts. You look up: the pit's sides are sheer hard dirt, about 15 feet deep. There are no roots, nothing down there with you besides dirt and whatever you have with you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to climb out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call for help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There's nothing to grab onto, but you dig your fingernails and toes into the dirt as best you can, trying to find rocks or roots to hold onto.
+You fall a few times, but you make progress. The pain in your leg blends with the pain in the rest of your body. Very slowly, you make your way to the top. Your fingers are bleeding, your wrists hurt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your voice rings out into the {location:current:type}. No one answers.
+After a few minutes, you hear skittering and see the squirrel peek its head into view. Then it disappears.
+A minute later, a vine woven from ferns and grasses drops down into the pit with you. The squirrel reappears, it's red eyes flashing, before it disappears again.
+You climb easily out of the pit. The squirrel is nowhere to be seen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWG1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;character:ranger&amp;location:current:forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As the sun sets, you see a small hut ahead of you, nestled between the trees. You pause, considering whether or not to investigate, but before you can decide, a group of men and women dressed like {character:ranger:name} steps out from behind the trees, surrounding you.
+"What are YOU doing here?" one of them asks you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask them what THEY are doing here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell them you're here to free {location:hometown:name} from {character:baron:baron} {character:baron:name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"We're fighting against the {character:baron:baron}'s influence, to free the villages {character:baron:subPronoun}'s conquered from {character:baron:possPronoun} control." You share that you're trying to do the same thing.
+You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
+They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
+In the morning, you set off for {location:baronhome:namewiththe} again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
+You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
+They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
+In the morning, you set off for {location:baronhome:namewiththe} again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As you head towards {location:baronhome:namewiththe}, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gather and enjoy some berries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid the patch and press on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You gather and eat some of the berries. They are delicious.
+You begin to feel sleepy, and soon fall asleep in the middle of the berry patch. When you wake up, the sun is high in the sky. You have no idea how long you've been asleep; it could have been days!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your stomach growls, but you continue on your way. As your food supply dwindles, your limbs grow weaker.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;item:map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;item:map&amp;character:stolen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character:baron&amp;character:stolen&amp;noitem:map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling {location:baronhome:namewiththe}. You think you can find a way in between them, but it would be tough. What do you do?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneak past the guards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take out one of the guards silently, then sneak inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside {location:baronhome:namewiththe} in the gap in the patrol.
+Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWF4</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -96,18 +406,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Set out for </t>
+      <t xml:space="preserve">character:baron</t>
     </r>
     <r>
       <rPr>
@@ -115,316 +414,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{location:baronhome:namewiththe}</t>
+      <t xml:space="preserve">&amp;noitem:map</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> immediately</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}
-The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You find a group of the {character:baron:baron}'s men in the tavern drinking. As one of them turns to you, your first blow lands squarely on his jaw. An all-out brawl breaks out. You give as good as you get, but in the end there are too many of them.
-"I'll take care of {objPronoun}," you hear a voice say. Rough hands carry you out of town into the nearby {location:nearby:name:pathtobaron}. You pass out.{|GOTO:pathtobaron|}
-You wake up the next day, deep in {location:current:namewiththe}. A {character:mentor:sexAge:ranger} sits under a nearby TREE. As you open your eyes, {character:ranger:subPronoun} says, "Hope you appreciate I saved your life. That was kind of a stupid fight to start, you know?"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character:baron&amp;character:ranger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
-"If you want to stop {character:baron:objPronoun} and get back {location:hometown:name}, you'll have to make it to {location:baronhome:namewiththe}."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ask {character:ranger:name} for {character:ranger:possPronoun} help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set off for {location:baronhome:namewiththe} (you know the way)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"I'm sorry, I can't go near the {character:baron:baron}'s </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{location:baronhome:type:cap}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> myself. {character:baron:subPronoun:cap} and {character:baron:possPronoun} goons'll be looking for me. But here, you take this." {character:ranger:subPronoun:cap} hands you piece of rolled cloth. "It might be useful." With that, {character:ranger:name} disappears into the {location:current:type}. {|GIVE:map:A cloth map:shows a hidden path into [location-baronhome-namewiththe]|}
-The cloth, once unrolled, looks like some sort of map of a secret entrance into the {character:baron:baron}'s </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{location:baronhome:type:cap}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. You roll it up again and put it in your pack.
-You travel through {location:current:namewiththe} for several days.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:baronhome:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
-You travel through {location:current:namewiththe} for several days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A wide river blocks your path to {location:baronhome:namewiththe}. The water is deep and moving fast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wade through the rushing water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Look for another way around</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
-It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
-Once you're ready, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
-On the other side, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOTW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character:baron&amp;character:ranger&amp;location:current:forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
-After a day or so, you hear footsteps crashing through the brush. They're getting nearer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hide in the brush and wait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seek out the footsteps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You find a clump of bushes to hide inside. As the footsteps get closer, you see two dozen of the {character:baron:baron}'s armed men tramping through the underbrush.
-You hold your breath, but one of them stumbles just too close to you.
-"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You tramp through the underbrush towards the sound of footsteps, getting closer as you hike. Then, through the trees, two dozen of the {character:baron:baron}'s men in uniform emerge.
-One of them grabs you roughly by the shoulder. "What do we have here?" he says. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOTW1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two more men grab your arms and bind them. You're taken to a camp in the woods an hour away. The {character:baron:baron}'s men tie you to a tree and spend the night drinking and making coarse jokes.
-Most of them have fallen asleep, but there is still one awake, on guard, staring into the fire. He isn't looking directly at you, you could try to escape while he isn't looking. What do you do?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wiggle out of your bonds and sneak into the night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wait until morning for a chance to escape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It takes you over an hour, but you eventually feel the bonds loosening enough that you can slip out of them. The lone guard is still staring into the fire, poking at it with his sword and humming.
-You grab your pack silently and disappear into the night, using the stars to head in the direction of {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
-Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip into the night.
-You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The next day, a small creature runs across your path. You almost step on it.
-You squat down to look at it. It seems like some sort of squirrel, but it's eyes are ruby red. It sits still, staring at you, alert.{|SET:squirrel:exists|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give it some of your food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The squirrel seems appreciative, and chirps happily. It looks deep into your eyes, then it scampers off into the {location:current:type}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The squirrel watches you as you leave, then scampers off.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Late in the day, you hear a voice calling out through the {location:current:type}. You hide immediately, but then realize the voice seems to be that of a young {character:child:sexAge:petowner}. You can see {character:petowner:objPronoun} walking alone, calling out for {character:petowner:possPronoun} cat. What do you do?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reveal yourself and offer to help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wait until {character:petowner:subPronoun}'s gone and continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You step out from behind your tree, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
-Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location:current:forest&amp;squirrel:exists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You're being careful, but you don't notice a well-concealed pit before it's too late. You step through the thin covering of leaves and ferns and fall right through to the bottom, landing with a crunch.
-Your leg hurts. You look up: the pit's sides are sheer hard dirt, about 15 feet deep. There are no roots, nothing down there with you besides dirt and whatever you have with you.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try to climb out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call for help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There's nothing to grab onto, but you dig your fingernails and toes into the dirt as best you can, trying to find rocks or roots to hold onto.
-You fall a few times, but you make progress. The pain in your leg blends with the pain in the rest of your body. Very slowly, you make your way to the top. Your fingers are bleeding, your wrists hurt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your voice rings out into the {location:current:type}. No one answers.
-After a few minutes, you hear skittering and see the squirrel peek its head into view. Then it disappears.
-A minute later, a vine woven from ferns and grasses drops down into the pit with you. The squirrel reappears, it's red eyes flashing, before it disappears again.
-You climb easily out of the pit. The squirrel is nowhere to be seen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As the sun sets, you see a small hut ahead of you, nestled between the trees. You pause, considering whether or not to investigate, but before you can decide, a group of men and women dressed like {character:ranger:name} steps out from behind the trees, surrounding you.
-"What are YOU doing here?" one of them asks you.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ask them what THEY are doing here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tell them you're here to free {location:hometown:name} from {character:baron:baron} {character:baron:name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"We're fighting against the {character:baron:baron}'s influence, to free the villages {character:baron:subPronoun}'s conquered from {character:baron:possPronoun} control." You share that you're trying to do the same thing.
-You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
-They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
-In the morning, you set off for {location:baronhome:namewiththe} again.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
-You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
-They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
-In the morning, you set off for {location:baronhome:namewiththe} again.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As you head towards {location:baronhome:namewiththe}, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gather and enjoy some berries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avoid the patch and press on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You gather and eat some of the berries. They are delicious.
-You begin to feel sleepy, and soon fall asleep in the middle of the berry patch. When you wake up, the sun is high in the sky. You have no idea how long you've been asleep; it could have been days!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your stomach growls, but you continue on your way. As your food supply dwindles, your limbs grow weaker.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character:baron&amp;item:map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character:baron&amp;item:map&amp;character:stolen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character:baron&amp;character:stolen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling {location:baronhome:namewiththe}. You think you can find a way in between them, but it would be tough. What do you do?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sneak past the guards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take out one of the guards silently, then sneak inside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
-Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumping out from your hiding place as a guard comes by, you take him out quickly and quietly. You drag the body behind a bush before quickly making your way inside {location:baronhome:namewiththe} in the gap in the patrol.
-Inside {location:baronhome:namewiththe}, you look around for any sign of {character:stolen:name}. While you're looking, you hear voices.{|AWF1a|}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWF4</t>
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
@@ -796,12 +787,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -899,16 +898,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="64.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1005,28 +1004,31 @@
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -1044,72 +1046,78 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>60</v>
@@ -1127,13 +1135,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C11" s="1" t="s">
         <v>66</v>
       </c>
@@ -1150,206 +1155,252 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a "goal", making conditions for the baron's journey super specific (not just "baron exists"), expanding on location conditions
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="138">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Go to work like always and see if anything changes</t>
   </si>
   <si>
-    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:name:pathtobaron}.{|GOTO:pathtobaron|}
+    <t xml:space="preserve">You set out for the {character:baron:baron}'s home, {location:fortress:namewiththe:baronhome}. You know the way, which leads through the nearby {location:nearby:name:pathtobaron}.{|GOTO:pathtobaron|}{|SET:goal:baronhome|}
 Deep in {location:current:namewiththe}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.{|MTM|}</t>
   </si>
   <si>
@@ -70,9 +70,25 @@
     <t xml:space="preserve">character:baron</t>
   </si>
   <si>
-    <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
 They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
 In the morning, your friend {character:bestfriend:name:stolen} is missing. {character:stolen:possPronoun:cap} family says that {character:stolen:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:fortress:name:baronhome} by {character:baron:possPronoun} men. They don't know when, or if, {character:stolen:subPronoun} will return.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{|SET:goal:baronhome|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Set out for {location:baronhome:namewiththe} immediately</t>
@@ -81,7 +97,7 @@
     <t xml:space="preserve">Start a fight with the {character:baron:baron}'s men</t>
   </si>
   <si>
-    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}
+    <t xml:space="preserve">You slink into the nearby {location:nearby:name:pathtobaron} in the night, setting your course straight for {location:goal:namewiththe}.{|GOTO:pathtobaron|}
 The next day, deep in the {location:current:type}, a {character:mentor:sexAge:ranger} emerges from behind the trees. {character:mentor:subPronoun:cap}'s wearing rough clothing.</t>
   </si>
   <si>
@@ -93,7 +109,7 @@
     <t xml:space="preserve">MTM1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;character:ranger</t>
+    <t xml:space="preserve">goal:baronhome&amp;character:ranger</t>
   </si>
   <si>
     <t xml:space="preserve">"My name's {character:ranger:name}," {character:ranger:subPronoun} says. "{location:hometown:name}'s not the first village that {character:baron:baron} {character:baron:name}'s taken control of. {character:baron:subPronoun:cap}'ll stop at nothing until the whole region is under {character:baron:possPronoun} control. We can't let that happen.
@@ -111,8 +127,33 @@
 You travel through {location:current:namewiththe} for several days.</t>
   </si>
   <si>
-    <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:baronhome:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You walk further into the {location:current:type}, headed for {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}. "Good luck with the {character:baron:baron}," {character:ranger:name} calls after you.
 You travel through {location:current:namewiththe} for several days.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CTT1</t>
@@ -121,7 +162,32 @@
     <t xml:space="preserve">location:current:forest</t>
   </si>
   <si>
-    <t xml:space="preserve">A wide river blocks your path to {location:baronhome:namewiththe}. The water is deep and moving fast.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A wide river blocks your path to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}. The water is deep and moving fast.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Wade through the rushing water</t>
@@ -130,19 +196,94 @@
     <t xml:space="preserve">Look for another way around</t>
   </si>
   <si>
-    <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You wade through the rushing water. It comes up to your armpits. You hold your pack above your head.
 It takes every ounce of your strength, but you make it across. On the other side, you're soaked to the bone and exhausted. You rest for an hour while your clothes dry.
-Once you're ready, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
-On the other side, you continue on your way to {location:baronhome:namewiththe}.</t>
+Once you're ready, you continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You walk along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
+On the other side, you continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CTT2</t>
   </si>
   <si>
-    <t xml:space="preserve">A tall wall runs across your path to {location:baronhome:namewiththe}. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A tall wall runs across your path to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}. Its stones are old and falling apart, but it might collapse on top of you if you try to climb it.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Climb the wall here</t>
@@ -151,34 +292,68 @@
     <t xml:space="preserve">Looking for a gap in the wall somewhere else</t>
   </si>
   <si>
-    <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
-You continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further along the wall, you find a tall tree with a branch leaning over the wall. You climb the tree, edge out along the branch, and drop down on the other side of the wall.
-Once over the wall, you continue on your way to {location:baronhome:namewiththe}.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You pull stones out of the wall as you climb, and they clatter to the ground below you. The wall shifts and sways as you climb, but miraculously doesn't collapse. When you get to the top and descend on the other side, you can hear stones skidding out of place behind you.
+You continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Further along the wall, you find a tall tree with a branch leaning over the wall. You climb the tree, edge out along the branch, and drop down on the other side of the wall.
+Once over the wall, you continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">BOTW1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">character:baron</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;character:ranger&amp;location:current:forest</t>
-    </r>
+    <t xml:space="preserve">goal:baronhome&amp;character:ranger&amp;location:current:forest</t>
   </si>
   <si>
     <t xml:space="preserve">Your path lies through a thick {location:current:type}, overgrown and difficult to travel through.
@@ -213,13 +388,63 @@
     <t xml:space="preserve">Wait until morning for a chance to escape</t>
   </si>
   <si>
-    <t xml:space="preserve">It takes you over an hour, but you eventually feel the bonds loosening enough that you can slip out of them. The lone guard is still staring into the fire, poking at it with his sword and humming.
-You grab your pack silently and disappear into the night, using the stars to head in the direction of {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">It takes you over an hour, but you eventually feel the bonds loosening enough that you can slip out of them. The lone guard is still staring into the fire, poking at it with his sword and humming.
+You grab your pack silently and disappear into the night, using the stars to head in the direction of {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You close your eyes and eventually fall into a fitful sleep.
 Hours later you feel someone removing your bonds. It's still night out. You turn to look and see {character:ranger:name}'s face. "Didn't think I'd find YOU when I came to investigate. Stay quiet." {character:ranger:subPronoun:cap} finishes cutting your bonds with {character:ranger:possPronoun} knife, and the two of you slip into the night.
-You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:baronhome:namewiththe}.</t>
+You travel for a few minutes away from the camp before you realize {character:ranger:name} is gone. The sun begins to rise as you silently make your way toward {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">BOTW2 </t>
@@ -275,11 +500,61 @@
     <t xml:space="preserve">Wait until {character:petowner:subPronoun}'s gone and continue</t>
   </si>
   <si>
-    <t xml:space="preserve">You step out from behind your tree, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
-Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to {location:baronhome:namewiththe}.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You step out from behind your tree, startling the {character:petowner:sexAge} briefly. {character:petowner:subPronoun:cap} seems thrilled to have the help. {character:petowner:subPronoun:cap} tells you {character:petowner:possPronoun} name is {character:petowner:name}, and {character:petowner:possPronoun} cat's name is Sniffles.
+Together, it takes you a few hours to find Sniffles. {character:petowner:name:cap} thanks you profusely for your help. Then, you continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{character:petowner:subPronoun:cap} continues calling and passes out of earshot in a few minutes. Then, you continue on your way to {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ROT3</t>
@@ -311,7 +586,23 @@
     <t xml:space="preserve">MWG1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;character:ranger&amp;location:current:forest</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;character:ranger&amp;location:current:forest</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">As the sun sets, you see a small hut ahead of you, nestled between the trees. You pause, considering whether or not to investigate, but before you can decide, a group of men and women dressed like {character:ranger:name} steps out from behind the trees, surrounding you.
@@ -324,22 +615,97 @@
     <t xml:space="preserve">Tell them you're here to free {location:hometown:name} from {character:baron:baron} {character:baron:name}</t>
   </si>
   <si>
-    <t xml:space="preserve">"We're fighting against the {character:baron:baron}'s influence, to free the villages {character:baron:subPronoun}'s conquered from {character:baron:possPronoun} control." You share that you're trying to do the same thing.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"We're fighting against the {character:baron:baron}'s influence, to free the villages {character:baron:subPronoun}'s conquered from {character:baron:possPronoun} control." You share that you're trying to do the same thing.
 You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
 They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
-In the morning, you set off for {location:baronhome:namewiththe} again.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
+In the morning, you set off for {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe} again.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"We're on the same side then! Have you met our friend {character:ranger:name}? {character:ranger:subPronoun:cap}'s out somewhere, fighting against the {character:baron:baron}'s influence."
 You spend the night with the resistance fighters. The {character:baron:baron}'s men, they tell you, are only working for {character:baron:objPronoun} because {character:baron:subPronoun} pays them handsomely. If you can find a way to stop the {character:baron:baron}'s men from being paid, most of {character:baron:possPronoun} influence over the region will be gone.
 They have plans to attack one of the {character:baron:baron}'s outposts tomorrow, which should draw most of {character:baron:possPronoun} men away from {location:baronhome:namewiththe}, allowing you to get inside more easily.
-In the morning, you set off for {location:baronhome:namewiththe} again.</t>
+In the morning, you set off for {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe} again.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">WAT1</t>
   </si>
   <si>
-    <t xml:space="preserve">As you head towards {location:baronhome:namewiththe}, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As you head towards {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}, late that day, on your left, you see a field of berry bushes, overflowing with red berries. Your food is running low, and you feel hungry.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Gather and enjoy some berries</t>
@@ -358,7 +724,23 @@
     <t xml:space="preserve">AWF1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;item:map</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;item:map</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}.{|AWF1a|}</t>
@@ -367,7 +749,23 @@
     <t xml:space="preserve">AWF2</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;item:map&amp;character:stolen</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;item:map&amp;character:stolen</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you find the hidden path into {location:baronhome:namewiththe} on {character:ranger:name}'s map. The hidden path leads underground, and comes out into a tall, well-decorated corridor inside {location:baronhome:namewiththe}. You look around for any sign of {character:stolen:name}.{|AWF1a|}</t>
@@ -376,7 +774,23 @@
     <t xml:space="preserve">AWF3</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;character:stolen&amp;noitem:map</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">goal:baronhome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;character:stolen&amp;noitem:map</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You finally arrive at the base of {location:baronhome:namewiththe}. Staying out of view of any of the {character:baron:baron}'s men, you look for a way in. There's a patrol of guards circling {location:baronhome:namewiththe}. You think you can find a way in between them, but it would be tough. What do you do?</t>
@@ -399,23 +813,7 @@
     <t xml:space="preserve">AWF4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">character:baron</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp;noitem:map</t>
-    </r>
+    <t xml:space="preserve">goal:baronhome&amp;noitem:map</t>
   </si>
   <si>
     <t xml:space="preserve">You have to wait until nightfall to sneak in. The cover of dark covers your movements, and you sneak in through a gap in the patrol you've found.
@@ -429,7 +827,7 @@
     <t xml:space="preserve">AWF1a</t>
   </si>
   <si>
-    <t xml:space="preserve">The {character:baron:baron} is walking down the hall with one of {character:baron:possPronoun} men. You find a place to hide, and you can hear them talking.
+    <t xml:space="preserve">{|GOTO:goal|}The {character:baron:baron} is walking down the hall with one of {character:baron:possPronoun} men. You find a place to hide, and you can hear them talking.
 "...if they resist, remind them that, if the kingdoms from the north attack, they will not be able to defend themselves. Under our rule, we will provide them with protection against invasion. What is that safety worth to them?..."
 The voices fade away as they turn a corner and are gone.</t>
   </si>
@@ -437,7 +835,7 @@
     <t xml:space="preserve">A1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:stolen&amp;character:baron</t>
+    <t xml:space="preserve">character:stolen&amp;location:current:baronhome</t>
   </si>
   <si>
     <t xml:space="preserve">You find {character:stolen:name} locked in a dungeon with a bunch of other young people. It seems they've been locked up here for some future purpose of the {character:baron:baron}. You set them all free.</t>
@@ -446,23 +844,52 @@
     <t xml:space="preserve">UB1</t>
   </si>
   <si>
-    <t xml:space="preserve">Searching in {location:baronhome:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside {location:baronhome:namewiththe}. The {character:baron:baron}'s gold is gone.</t>
+    <t xml:space="preserve">location:current:baronhome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching in {location:current:namewiththe}, you finally find the treasury. You take out the lone guard, and go inside. Several heavy chests of gold are inside. You dump them out the window into a lake outside {location:current:namewiththe}. The {character:baron:baron}'s gold is gone.</t>
   </si>
   <si>
     <t xml:space="preserve">ROR1</t>
   </si>
   <si>
-    <t xml:space="preserve">You leave {location:baronhome:namewiththe}.{|GOTO:pathtobaron|}</t>
+    <t xml:space="preserve">You leave {location:current:namewiththe}.{|SET:goal:hometown|}</t>
   </si>
   <si>
     <t xml:space="preserve">MF1</t>
   </si>
   <si>
-    <t xml:space="preserve">character:baron&amp;location:current:forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:current:type} as fast as you can.
-The {character:baron:baron}'s men are chasing you through {location:pathtobaron:namewiththe} on your way back to {location:hometown:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
+    <t xml:space="preserve">location:current:baronhome&amp;location:pathtobaron:forest&amp;goal:hometown</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As you leave, {character:baron:baron} {character:baron:name} spots you leaving. "After {objPronoun}!" {character:baron:subPronoun} shouts to {character:baron:possPronoun} men, and they begin to chase after you. You sprint into the {location:current:type} as fast as you can.{|SET:chasedbybaron:true|}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{|GOTO:pathtobaron|}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+The {character:baron:baron}'s men are chasing you through {location:current:namewiththe} on your way back to {location:goal:name}. If they catch you, there's no telling what they might do to you. To avoid notice, you...</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Spend your nights well-hidden, in a hole or under heavy brush</t>
@@ -472,11 +899,11 @@
   </si>
   <si>
     <t xml:space="preserve">Your nights are uncomfortable. You wake up each morning covered in dirt or leaves or both.
-One night, you're woken in the middle of the night by the sound of men's footsteps. The {character:baron:baron}'s men are searching the {location:pathtobaron:name} for you. They almost find your hiding spot, but you hear skittering in the trees, and the {character:baron:baron}'s men go off to investigate the sound. You see a flash of red in the trees, possibly two eyes looking at you, and then it's gone.
+One night, you're woken in the middle of the night by the sound of men's footsteps. The {character:baron:baron}'s men are searching {location:current:namewiththe} for you. They almost find your hiding spot, but you hear skittering in the trees, and the {character:baron:baron}'s men go off to investigate the sound. You see a flash of red in the trees, possibly two eyes looking at you, and then it's gone.
 You keep going, and you manage to stay ahead of the {character:baron:baron}'s men.</t>
   </si>
   <si>
-    <t xml:space="preserve">You push on through the night. You're exhausted by the time you reach {location:hometown:name}, but you are ahead of the {character:baron:baron}'s men.</t>
+    <t xml:space="preserve">You push on through the night. You're exhausted by the time you reach {location:goal:name}, but you are ahead of the {character:baron:baron}'s men.</t>
   </si>
   <si>
     <t xml:space="preserve">RFW1</t>
@@ -485,20 +912,92 @@
     <t xml:space="preserve">CRT1</t>
   </si>
   <si>
-    <t xml:space="preserve">You finally return to {location:hometown:name}. The people have been under the rule of the {character:baron:baron}'s men since you left, who have done nothing but drink and destroy property that isn't theirs. The men pursuing you are close behind, maybe a day or so.</t>
+    <t xml:space="preserve">chasedbybaron:true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{|GOTO:hometown|}You finally return to {location:current:name}. The people have been under the rule of the {character:baron:baron}'s men since you left, who have done nothing but drink and destroy property that isn't theirs. The men pursuing you are close behind, maybe a day or so.</t>
   </si>
   <si>
     <t xml:space="preserve">MOTW1</t>
   </si>
   <si>
-    <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:hometown:name}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.
-The next day, the men who were pursuing you arrive. {location:hometown:name}'s finest easily chases them off; there is strength in numbers, and they knew what to expect, thanks to you.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You organize a secret meeting at night to rally the people together. You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they retreat, leaving the town forever.
+The next day, the men who were pursuing you arrive. {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">current</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe:cap}'s finest easily chases them off. There is strength in numbers, and they knew what to expect, thanks to you.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
   </si>
   <si>
-    <t xml:space="preserve">{location:hometown:name} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the Chief of {location:hometown:name}. What do you do?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">chasedbybaron:true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;location:current:hometown</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{location:hometown:namewiththe:cap} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the Chief of {location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">hometown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:namewiththe}. What do you do? {|SET:chasedbybaron:false|}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Go back to your old job, {industry:hometown:workGer}</t>
@@ -796,11 +1295,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -900,8 +1399,8 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,7 +1499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1549,7 @@
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1090,10 +1589,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1116,7 +1615,7 @@
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1182,7 +1681,7 @@
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1225,7 +1724,7 @@
       <c r="A15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1236,7 +1735,7 @@
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1247,7 +1746,7 @@
       <c r="A17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1270,7 +1769,7 @@
       <c r="A18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1297,7 +1796,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>110</v>
       </c>
@@ -1312,95 +1811,95 @@
       <c r="A21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
+      <c r="B21" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>116</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>14</v>
+        <v>131</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding "chief"/"chieftess"; adding city templates from Louisa and writing new industries
</commit_message>
<xml_diff>
--- a/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
+++ b/NeverendingStory/NeverendingStory.Console/Scenes.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">location:current:hometown</t>
   </si>
   <si>
-    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, bringing back enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
+    <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, {industry:hometown:goodsGer} enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
 One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {character:antagonist:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."
 What do you do?</t>
   </si>
@@ -597,13 +597,13 @@
     <t xml:space="preserve">chasedbybaron:true&amp;location:current:hometown</t>
   </si>
   <si>
-    <t xml:space="preserve">{location:hometown:namewiththe:cap} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the Chief of {location:hometown:namewiththe}. What do you do? {|SET:chasedbybaron:false|}</t>
+    <t xml:space="preserve">{location:hometown:namewiththe:cap} is now free! Your fellow citizens are eagerly offering you a position of leadership: they want to make you the {chief} of {location:hometown:namewiththe}. What do you do? {|SET:chasedbybaron:false|}</t>
   </si>
   <si>
     <t xml:space="preserve">Go back to your old job, {industry:hometown:workGer}</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the new job as Chief of {location:hometown:name}</t>
+    <t xml:space="preserve">Take the new job as {chief} of {location:hometown:name}</t>
   </si>
   <si>
     <t xml:space="preserve">{industry:hometown:gooddayfinal} {location:hometown:name}'s freedom allows things to go back to the way that they were. But you know that, if ever another {character:baron:baron} tried to take control of {location:hometown:name} again, you and your neighbors would be ready for them.</t>
@@ -995,8 +995,8 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1029,7 +1029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>